<commit_message>
metadata updates & reorder phosphate and silicate
</commit_message>
<xml_diff>
--- a/nutrient-mvco-info.xlsx
+++ b/nutrient-mvco-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4247343-AD84-43CA-8CAF-7BF6B8FB7633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D56D38-F2D0-4516-9307-B25E6894197F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30885" yWindow="6105" windowWidth="25125" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="96">
   <si>
     <t>attributeName</t>
   </si>
@@ -252,15 +252,9 @@
     <t>contact</t>
   </si>
   <si>
-    <t>Ammonium concentration in the water column</t>
-  </si>
-  <si>
     <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
   <si>
-    <t>Date and time in UTC when rosette bottle closed or bucket filled</t>
-  </si>
-  <si>
     <t>datetime</t>
   </si>
   <si>
@@ -273,19 +267,55 @@
     <t>Lowercase letter indicating replicate subsample drawn from the same rosette bottle or bucket</t>
   </si>
   <si>
-    <t>Ship's latitude when rosette bottle closed or bucket filled</t>
-  </si>
-  <si>
-    <t>Ship's longitude when rosette bottle closed or bucket filled</t>
-  </si>
-  <si>
     <t>PI</t>
   </si>
   <si>
     <t>Code identifying event number for day cruises to MVCO.</t>
   </si>
   <si>
-    <t>Code in general identifying event number and Niskin for day cruises to MVCO.</t>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Peacock</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Morkeski</t>
+  </si>
+  <si>
+    <t>metadataProvider</t>
+  </si>
+  <si>
+    <t>0000-0002-2903-5851</t>
+  </si>
+  <si>
+    <t>kmorkeski@whoi.edu</t>
+  </si>
+  <si>
+    <t>epeacock@whoi.edu</t>
+  </si>
+  <si>
+    <t>ecrockford@whoi.edu</t>
+  </si>
+  <si>
+    <t>inorganic matter</t>
+  </si>
+  <si>
+    <t>Code in general identifying event number and Niskin (and collaborating institution) for day cruises to MVCO.</t>
+  </si>
+  <si>
+    <t>Date and time in UTC when cast started or bucket filled</t>
+  </si>
+  <si>
+    <t>Ship's latitude when cast started or bucket filled</t>
+  </si>
+  <si>
+    <t>Ship's longitude when cast started or bucket filled</t>
+  </si>
+  <si>
+    <t>Ammonium concentration in the water column URI http://vocab.nerc.ac.uk/collection/P02/current/AMON/</t>
   </si>
 </sst>
 </file>
@@ -328,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -337,6 +367,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,7 +651,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,10 +686,10 @@
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -672,10 +703,10 @@
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -689,16 +720,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -712,7 +743,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -732,7 +763,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -772,7 +803,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -804,12 +835,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -826,10 +857,10 @@
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -846,10 +877,10 @@
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -872,10 +903,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9F15A2-54C5-8A40-9C46-AA79FB7AA201}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,7 +998,7 @@
         <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
         <v>62</v>
@@ -989,6 +1020,9 @@
       <c r="D4" t="s">
         <v>62</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="G4" t="s">
         <v>70</v>
       </c>
@@ -1004,16 +1038,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
       </c>
       <c r="D5" t="s">
         <v>62</v>
       </c>
-      <c r="E5" t="s">
-        <v>72</v>
+      <c r="E5" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
         <v>62</v>
@@ -1022,6 +1059,58 @@
         <v>65</v>
       </c>
       <c r="J5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1034,13 +1123,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8891376B-2E72-9645-AC2E-5AA2D44D3942}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1053,7 +1143,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
added transformation & map checks and updated methods
</commit_message>
<xml_diff>
--- a/nutrient-mvco-info.xlsx
+++ b/nutrient-mvco-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D56D38-F2D0-4516-9307-B25E6894197F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D432F373-9C00-4D48-8FC6-272CE6633735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32010" yWindow="5940" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Phosphate concentration in the water column. URI http://vocab.nerc.ac.uk/collection/P02/current/PHOS/</t>
   </si>
   <si>
-    <t>Silicate concentration in the water column. URI http://vocab.nerc.ac.uk/collection/P02/current/SLCA/</t>
-  </si>
-  <si>
     <t>Depth of sample below sea surface. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>PI</t>
   </si>
   <si>
-    <t>Code identifying event number for day cruises to MVCO.</t>
-  </si>
-  <si>
     <t>Emily</t>
   </si>
   <si>
@@ -303,26 +297,32 @@
     <t>inorganic matter</t>
   </si>
   <si>
-    <t>Code in general identifying event number and Niskin (and collaborating institution) for day cruises to MVCO.</t>
-  </si>
-  <si>
     <t>Date and time in UTC when cast started or bucket filled</t>
   </si>
   <si>
-    <t>Ship's latitude when cast started or bucket filled</t>
-  </si>
-  <si>
-    <t>Ship's longitude when cast started or bucket filled</t>
-  </si>
-  <si>
     <t>Ammonium concentration in the water column URI http://vocab.nerc.ac.uk/collection/P02/current/AMON/</t>
+  </si>
+  <si>
+    <t>Latitude of the MVCO or ship's latitude when cast started or bucket filled</t>
+  </si>
+  <si>
+    <t>Code identfiying event number and Niskin or bucket sample</t>
+  </si>
+  <si>
+    <t>Longitude of the MVCO or ship's longitude when cast started or bucket filled</t>
+  </si>
+  <si>
+    <t>Code identifying event number for day cruises to MVCO</t>
+  </si>
+  <si>
+    <t>Silicate concentration in the water column URI http://vocab.nerc.ac.uk/collection/P02/current/SLCA/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +332,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -358,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -368,6 +375,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,16 +656,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="62.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="90" style="1" customWidth="1"/>
     <col min="3" max="8" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -684,35 +692,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>91</v>
+        <v>76</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -720,19 +728,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -743,16 +751,16 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -763,16 +771,16 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -783,16 +791,16 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
         <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -803,13 +811,13 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -820,16 +828,16 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -840,16 +848,16 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -866,34 +874,37 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -916,202 +927,202 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>57</v>
-      </c>
-      <c r="J1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>62</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
         <v>64</v>
       </c>
-      <c r="G2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>65</v>
-      </c>
-      <c r="J2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
         <v>59</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>61</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>63</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
         <v>64</v>
       </c>
-      <c r="G3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>65</v>
-      </c>
-      <c r="J3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" t="s">
-        <v>70</v>
-      </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
         <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" t="s">
         <v>65</v>
-      </c>
-      <c r="J5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>72</v>
       </c>
-      <c r="G6" t="s">
-        <v>73</v>
-      </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" t="s">
         <v>65</v>
-      </c>
-      <c r="J6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" t="s">
         <v>83</v>
       </c>
-      <c r="C7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" t="s">
-        <v>85</v>
-      </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" t="s">
         <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1135,66 +1146,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1202,23 +1213,23 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1226,15 +1237,15 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1254,36 +1265,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
       </c>
       <c r="D2">
         <v>1E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ship and cruise identifiers
</commit_message>
<xml_diff>
--- a/nutrient-mvco-info.xlsx
+++ b/nutrient-mvco-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D432F373-9C00-4D48-8FC6-272CE6633735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD51B8F7-D67A-4254-BF06-ECC6B952E832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32010" yWindow="5940" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
   <si>
     <t>attributeName</t>
   </si>
@@ -316,6 +316,18 @@
   </si>
   <si>
     <t>Silicate concentration in the water column URI http://vocab.nerc.ac.uk/collection/P02/current/SLCA/</t>
+  </si>
+  <si>
+    <t>ship</t>
+  </si>
+  <si>
+    <t>cruise_ID</t>
+  </si>
+  <si>
+    <t>Name of vessel from which samples were collected</t>
+  </si>
+  <si>
+    <t>Cruise identifer for the R/V Tioga</t>
   </si>
 </sst>
 </file>
@@ -656,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,56 +740,38 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -786,18 +780,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
@@ -806,15 +800,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -825,16 +822,16 @@
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
@@ -845,16 +842,13 @@
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
         <v>24</v>
@@ -865,10 +859,10 @@
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -883,12 +877,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -903,8 +897,48 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
round lat/long, update creators & geographic desc
</commit_message>
<xml_diff>
--- a/nutrient-mvco-info.xlsx
+++ b/nutrient-mvco-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD51B8F7-D67A-4254-BF06-ECC6B952E832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C344F70B-0B10-4571-B213-42121453BADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28764" yWindow="-1524" windowWidth="21552" windowHeight="11784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="99">
   <si>
     <t>attributeName</t>
   </si>
@@ -102,9 +102,6 @@
     <t>meter</t>
   </si>
   <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>micromolePerLiter</t>
   </si>
   <si>
@@ -237,9 +234,6 @@
     <t>Crockford</t>
   </si>
   <si>
-    <t>technician</t>
-  </si>
-  <si>
     <t>NES-LTER Information Manager</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
     <t>Morkeski</t>
   </si>
   <si>
-    <t>metadataProvider</t>
-  </si>
-  <si>
     <t>0000-0002-2903-5851</t>
   </si>
   <si>
@@ -328,6 +319,12 @@
   </si>
   <si>
     <t>Cruise identifer for the R/V Tioga</t>
+  </si>
+  <si>
+    <t>Metadata Provider</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -670,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,16 +703,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -723,16 +720,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -740,10 +737,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -751,10 +748,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -762,19 +759,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -785,7 +782,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -794,7 +791,7 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -805,7 +802,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -814,7 +811,7 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -834,7 +831,7 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -845,13 +842,13 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -868,10 +865,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -882,16 +879,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -908,10 +905,10 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -922,16 +919,16 @@
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -951,7 +948,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,202 +958,202 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>55</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>56</v>
-      </c>
-      <c r="J1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>61</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
         <v>63</v>
       </c>
-      <c r="G2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>64</v>
-      </c>
-      <c r="J2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>60</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>61</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>62</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
         <v>63</v>
       </c>
-      <c r="G3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
         <v>64</v>
-      </c>
-      <c r="J4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" t="s">
         <v>64</v>
-      </c>
-      <c r="J5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
         <v>70</v>
       </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s">
         <v>64</v>
-      </c>
-      <c r="J6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" t="s">
         <v>81</v>
       </c>
-      <c r="C7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" t="s">
-        <v>84</v>
-      </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" t="s">
         <v>64</v>
-      </c>
-      <c r="J7" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1180,66 +1177,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1247,23 +1244,23 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1271,15 +1268,15 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1299,36 +1296,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
       </c>
       <c r="D2">
         <v>1E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits from ETC comments
</commit_message>
<xml_diff>
--- a/nutrient-mvco-info.xlsx
+++ b/nutrient-mvco-info.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C344F70B-0B10-4571-B213-42121453BADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F79556B-A326-47CE-98D5-5A03DB3821A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28764" yWindow="-1524" windowWidth="21552" windowHeight="11784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30660" yWindow="-4416" windowWidth="15312" windowHeight="16644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
     <sheet name="Personnel" sheetId="2" r:id="rId2"/>
     <sheet name="Keywords" sheetId="3" r:id="rId3"/>
     <sheet name="CustomUnits" sheetId="4" r:id="rId4"/>
+    <sheet name="CategoricalVariables" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
   <si>
     <t>attributeName</t>
   </si>
@@ -294,18 +295,6 @@
     <t>Ammonium concentration in the water column URI http://vocab.nerc.ac.uk/collection/P02/current/AMON/</t>
   </si>
   <si>
-    <t>Latitude of the MVCO or ship's latitude when cast started or bucket filled</t>
-  </si>
-  <si>
-    <t>Code identfiying event number and Niskin or bucket sample</t>
-  </si>
-  <si>
-    <t>Longitude of the MVCO or ship's longitude when cast started or bucket filled</t>
-  </si>
-  <si>
-    <t>Code identifying event number for day cruises to MVCO</t>
-  </si>
-  <si>
     <t>Silicate concentration in the water column URI http://vocab.nerc.ac.uk/collection/P02/current/SLCA/</t>
   </si>
   <si>
@@ -325,13 +314,46 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>IODE Quality Flag primary level</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>iode_quality_flag_phosphate</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>questionable/suspect</t>
+  </si>
+  <si>
+    <t>Ship's latitude when cast started or latitude of MVCO</t>
+  </si>
+  <si>
+    <t>Ship's longitude when cast started or longitude of MVCO</t>
+  </si>
+  <si>
+    <t>Identification number for each MVCO discrete sampling event</t>
+  </si>
+  <si>
+    <t>Identification number for each Niskin or bucket collection during MVCO discrete sampling event</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,8 +369,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF333333"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -371,10 +400,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -384,10 +414,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{9220847D-AE6F-4AA0-9CCD-855E6C2DDD8F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -667,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,14 +740,14 @@
       <c r="A2" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>91</v>
+      <c r="B2" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -722,14 +757,14 @@
       <c r="A3" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>89</v>
+      <c r="B3" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -737,10 +772,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -748,10 +783,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -771,7 +806,7 @@
         <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -782,7 +817,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -791,7 +826,7 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -802,7 +837,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -811,7 +846,7 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -831,7 +866,7 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -848,7 +883,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -868,7 +903,7 @@
         <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -888,18 +923,18 @@
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -908,18 +943,18 @@
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -928,10 +963,21 @@
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -948,7 +994,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,7 +1190,7 @@
         <v>81</v>
       </c>
       <c r="G7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H7" t="s">
         <v>60</v>
@@ -1331,4 +1377,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A38778-F0CA-402D-99CD-D18D063CB2DF}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="12.44140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merge MVCO samples from transect cruises
</commit_message>
<xml_diff>
--- a/nutrient-mvco-info.xlsx
+++ b/nutrient-mvco-info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkoch\Desktop\LTER\nes-lter-nutrient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F79556B-A326-47CE-98D5-5A03DB3821A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD28B82-7026-4648-BEC5-4F98EBA76EBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30660" yWindow="-4416" windowWidth="15312" windowHeight="16644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="107">
   <si>
     <t>attributeName</t>
   </si>
@@ -313,9 +313,6 @@
     <t>Metadata Provider</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>IODE Quality Flag primary level</t>
   </si>
   <si>
@@ -347,6 +344,12 @@
   </si>
   <si>
     <t>Identification number for each Niskin or bucket collection during MVCO discrete sampling event</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -702,18 +705,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.41796875" customWidth="1"/>
     <col min="2" max="2" width="90" style="1" customWidth="1"/>
-    <col min="3" max="8" width="20.44140625" customWidth="1"/>
+    <col min="3" max="8" width="20.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -736,41 +739,41 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>74</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -780,8 +783,14 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -792,7 +801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -806,18 +815,18 @@
         <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -826,18 +835,18 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -846,13 +855,13 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -866,13 +875,13 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -883,13 +892,13 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -903,13 +912,13 @@
         <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -923,13 +932,13 @@
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -943,13 +952,13 @@
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -963,24 +972,24 @@
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B21" s="3"/>
     </row>
   </sheetData>
@@ -997,12 +1006,12 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1066,7 +1075,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1098,7 +1107,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -1124,7 +1133,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1150,7 +1159,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1173,7 +1182,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1215,13 +1224,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.7890625" customWidth="1"/>
+    <col min="2" max="2" width="40.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1229,7 +1238,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -1237,7 +1246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -1245,7 +1254,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1253,7 +1262,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1261,7 +1270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -1269,7 +1278,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1277,7 +1286,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -1285,7 +1294,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1293,7 +1302,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1301,7 +1310,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1309,7 +1318,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1317,7 +1326,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1338,9 +1347,9 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1357,7 +1366,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1387,45 +1396,45 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.41796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="12.44140625" style="5"/>
+    <col min="1" max="1" width="27.1015625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.68359375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.1015625" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="12.41796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="5">
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename cruise col, convert txt to md
</commit_message>
<xml_diff>
--- a/nutrient-mvco-info.xlsx
+++ b/nutrient-mvco-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7657EE-37E0-4D17-B659-1EC6CF4536AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6883093C-A392-48EF-8C0D-28FF723A1250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7692" yWindow="228" windowWidth="15156" windowHeight="12024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -264,9 +264,6 @@
     <t>ship</t>
   </si>
   <si>
-    <t>cruise_ID</t>
-  </si>
-  <si>
     <t>Name of vessel from which samples were collected</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>Identification number for each bucket collection (suffix _00) or rosette bottle (suffix greater than 0)</t>
+  </si>
+  <si>
+    <t>cruise</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,16 +712,16 @@
         <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -729,16 +729,16 @@
         <v>66</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -746,24 +746,24 @@
         <v>77</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -783,10 +783,10 @@
         <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -803,7 +803,7 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -814,7 +814,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -823,7 +823,7 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -843,7 +843,7 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -860,10 +860,10 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -880,7 +880,7 @@
         <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -900,7 +900,7 @@
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -920,7 +920,7 @@
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -940,7 +940,7 @@
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -948,13 +948,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1089,7 +1089,7 @@
         <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G4" t="s">
         <v>57</v>
@@ -1118,7 +1118,7 @@
         <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G5" t="s">
         <v>57</v>
@@ -1305,43 +1305,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update input data, rename date column
</commit_message>
<xml_diff>
--- a/nutrient-mvco-info.xlsx
+++ b/nutrient-mvco-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6883093C-A392-48EF-8C0D-28FF723A1250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B29A38-CF49-4913-A1AE-6C610EBA87C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
   <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>event_number</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>cruise</t>
+  </si>
+  <si>
+    <t>date_time_utc</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,61 +709,61 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -771,10 +771,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -783,10 +783,10 @@
         <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -803,7 +803,7 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -814,7 +814,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -823,7 +823,7 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -843,7 +843,7 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -854,16 +854,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -880,7 +880,7 @@
         <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -891,7 +891,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -900,7 +900,7 @@
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -911,7 +911,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -920,7 +920,7 @@
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -940,7 +940,7 @@
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -948,13 +948,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1063,7 +1063,7 @@
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
         <v>52</v>
@@ -1086,10 +1086,10 @@
         <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" t="s">
         <v>57</v>
@@ -1106,19 +1106,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
         <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
         <v>57</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -1305,43 +1305,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>